<commit_message>
setup buttons visible by the role
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/workflow.xlsx
+++ b/src/main/webapp/WEB-INF/book/workflow.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
+    <workbookView xWindow="5120" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>employee</t>
   </si>
@@ -45,15 +45,30 @@
   <si>
     <t>Please select a submission:</t>
   </si>
+  <si>
+    <t>Smart HR System</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Form</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Last Update</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -89,9 +104,19 @@
       <name val="Helvetica"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="72"/>
-      <name val="Helvetica"/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -114,17 +139,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -157,16 +190,16 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor>
         <xdr:from>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>812800</xdr:colOff>
-          <xdr:row>3</xdr:row>
-          <xdr:rowOff>25400</xdr:rowOff>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>12700</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>812800</xdr:colOff>
-          <xdr:row>3</xdr:row>
-          <xdr:rowOff>419100</xdr:rowOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>12700</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>406400</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -262,8 +295,8 @@
             <a:noFill/>
             <a:ln w="9525">
               <a:miter lim="800000"/>
-              <a:headEnd type="none" w="med" len="med"/>
-              <a:tailEnd type="none" w="med" len="med"/>
+              <a:headEnd/>
+              <a:tailEnd/>
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
@@ -301,13 +334,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor>
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>0</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>4</xdr:col>
+          <xdr:col>5</xdr:col>
           <xdr:colOff>25400</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
@@ -334,8 +367,8 @@
             <a:noFill/>
             <a:ln w="9525">
               <a:miter lim="800000"/>
-              <a:headEnd type="none" w="med" len="med"/>
-              <a:tailEnd type="none" w="med" len="med"/>
+              <a:headEnd/>
+              <a:tailEnd/>
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
@@ -630,32 +663,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="2:5" ht="47" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:5" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:5" ht="34" x14ac:dyDescent="0.4">
-      <c r="D2" s="4" t="s">
+    <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.4">
+      <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="C3" s="6"/>
     </row>
-    <row r="4" spans="2:5" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:5" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D2:E2"/>
+  <mergeCells count="2">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
       <formula1>"employee, supervisor"</formula1>
     </dataValidation>
   </dataValidations>
@@ -671,16 +714,16 @@
               <controlPr defaultSize="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
-                    <xdr:colOff>812800</xdr:colOff>
-                    <xdr:row>3</xdr:row>
-                    <xdr:rowOff>25400</xdr:rowOff>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>12700</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>4</xdr:col>
-                    <xdr:colOff>812800</xdr:colOff>
-                    <xdr:row>3</xdr:row>
-                    <xdr:rowOff>419100</xdr:rowOff>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>12700</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>406400</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -707,7 +750,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -751,30 +794,46 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.1640625" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.5" style="6" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="25.1640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="3"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -788,13 +847,13 @@
               <controlPr defaultSize="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>4</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>0</xdr:row>
                     <xdr:rowOff>25400</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>4</xdr:col>
+                    <xdr:col>5</xdr:col>
                     <xdr:colOff>25400</xdr:colOff>
                     <xdr:row>1</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>

</xml_diff>

<commit_message>
add state column, enable filter
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/workflow.xlsx
+++ b/src/main/webapp/WEB-INF/book/workflow.xlsx
@@ -18,6 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'form list'!$C$3:$D$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'submission list'!$A$3:$E$3</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>employee</t>
   </si>
@@ -59,6 +60,9 @@
   </si>
   <si>
     <t>Please select a form below:</t>
+  </si>
+  <si>
+    <t>State</t>
   </si>
 </sst>
 </file>
@@ -334,13 +338,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor>
         <xdr:from>
-          <xdr:col>4</xdr:col>
+          <xdr:col>5</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>25400</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
@@ -666,7 +670,7 @@
   <dimension ref="A2:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E2"/>
+      <selection activeCell="B4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -743,7 +747,7 @@
   <dimension ref="A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -796,30 +800,31 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E3"/>
+  <dimension ref="A2:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.1640625" style="4" customWidth="1"/>
     <col min="2" max="2" width="28.6640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="18.83203125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="25.1640625" style="3" customWidth="1"/>
+    <col min="3" max="4" width="18.83203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="25.1640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
-      <c r="E2" s="2"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
@@ -829,13 +834,17 @@
       <c r="C3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A3:E3"/>
   <mergeCells count="1">
-    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -849,13 +858,13 @@
               <controlPr defaultSize="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
-                    <xdr:col>4</xdr:col>
+                    <xdr:col>5</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>1</xdr:row>
                     <xdr:rowOff>25400</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>25400</xdr:colOff>
                     <xdr:row>2</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>

</xml_diff>

<commit_message>
Chaptalized the login role
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/workflow.xlsx
+++ b/src/main/webapp/WEB-INF/book/workflow.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6220" yWindow="4820" windowWidth="20380" windowHeight="10020" tabRatio="500"/>
+    <workbookView xWindow="37800" yWindow="3940" windowWidth="23420" windowHeight="10020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
     <t>Status</t>
   </si>
   <si>
-    <t>employee</t>
+    <t>Employee</t>
   </si>
 </sst>
 </file>
@@ -1122,15 +1122,14 @@
       <c r="I12" s="13"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="3">
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="D4:F4"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6">
-      <formula1>"employee, supervisor"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:F6">
+      <formula1>"Employee, Supervisor"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
rename buttons: login --> enter logout --> leave
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/workflow.xlsx
+++ b/src/main/webapp/WEB-INF/book/workflow.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="37800" yWindow="3940" windowWidth="23420" windowHeight="10020" tabRatio="500"/>
+    <workbookView xWindow="8040" yWindow="1900" windowWidth="23460" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="login" sheetId="2" r:id="rId1"/>
+    <sheet name="main" sheetId="2" r:id="rId1"/>
     <sheet name="form list" sheetId="1" state="hidden" r:id="rId2"/>
     <sheet name="submission list" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
@@ -509,7 +509,7 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1026" name="login" hidden="1">
+            <xdr:cNvPr id="1026" name="enter" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1026"/>
@@ -549,7 +549,7 @@
                   <a:ea typeface="Helvetica"/>
                   <a:cs typeface="Helvetica"/>
                 </a:rPr>
-                <a:t>Login</a:t>
+                <a:t>Enter</a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
@@ -581,7 +581,7 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="2049" name="logout" hidden="1">
+            <xdr:cNvPr id="2049" name="leave" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2049"/>
@@ -621,7 +621,7 @@
                   <a:ea typeface="Helvetica"/>
                   <a:cs typeface="Helvetica"/>
                 </a:rPr>
-                <a:t>Logout</a:t>
+                <a:t>Leave</a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
@@ -653,7 +653,7 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="3073" name="logout" hidden="1">
+            <xdr:cNvPr id="3073" name="leave" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3073"/>
@@ -693,7 +693,7 @@
                   <a:ea typeface="Helvetica"/>
                   <a:cs typeface="Helvetica"/>
                 </a:rPr>
-                <a:t>Logout</a:t>
+                <a:t>Leave</a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
@@ -1141,7 +1141,7 @@
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1026" r:id="rId3" name="login">
+            <control shapeId="1026" r:id="rId3" name="enter">
               <controlPr defaultSize="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
@@ -1174,7 +1174,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1321,7 +1321,7 @@
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2049" r:id="rId3" name="logout">
+            <control shapeId="2049" r:id="rId3" name="leave">
               <controlPr defaultSize="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
@@ -1354,7 +1354,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="135" zoomScaleNormal="135" zoomScalePageLayoutView="135" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1555,7 +1555,7 @@
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3073" r:id="rId3" name="logout">
+            <control shapeId="3073" r:id="rId3" name="leave">
               <controlPr defaultSize="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>

</xml_diff>

<commit_message>
* improve form file names and use them as item list without ".xlsx" * make submission list center align
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/workflow.xlsx
+++ b/src/main/webapp/WEB-INF/book/workflow.xlsx
@@ -292,18 +292,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -337,17 +325,29 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -369,7 +369,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="15">
     <dxf>
       <font>
         <b val="0"/>
@@ -393,7 +393,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
     <dxf>
       <font>
@@ -417,7 +417,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
     <dxf>
       <font>
@@ -442,7 +442,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
     <dxf>
       <font>
@@ -467,7 +467,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
     <dxf>
       <font>
@@ -492,7 +492,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
     <dxf>
       <font>
@@ -516,7 +516,10 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
     <dxf>
       <font>
@@ -638,11 +641,11 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7">
     <tableStyle name="Table Style 2" pivot="0" count="5">
-      <tableStyleElement type="wholeTable" dxfId="13"/>
-      <tableStyleElement type="headerRow" dxfId="12"/>
-      <tableStyleElement type="firstRowStripe" dxfId="11"/>
-      <tableStyleElement type="secondRowStripe" dxfId="10"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="9"/>
+      <tableStyleElement type="wholeTable" dxfId="14"/>
+      <tableStyleElement type="headerRow" dxfId="13"/>
+      <tableStyleElement type="firstRowStripe" dxfId="12"/>
+      <tableStyleElement type="secondRowStripe" dxfId="11"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="10"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -889,16 +892,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table64" displayName="Table64" ref="C5:C12" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table64" displayName="Table64" ref="C5:C12" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <tableColumns count="1">
-    <tableColumn id="1" name="Name" dataDxfId="6"/>
+    <tableColumn id="1" name="Name" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="C5:G7" totalsRowShown="0" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="C5:G7" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="C5:G7"/>
   <tableColumns count="5">
     <tableColumn id="1" name="ID" dataDxfId="4"/>
@@ -1408,7 +1411,7 @@
   <dimension ref="B1:I29"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1425,53 +1428,53 @@
       <c r="E1" s="14"/>
     </row>
     <row r="2" spans="2:9" s="6" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="32"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="29"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="25"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
       <c r="I2" s="15"/>
     </row>
     <row r="3" spans="2:9" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="32"/>
-      <c r="C3" s="36" t="s">
+      <c r="B3" s="28"/>
+      <c r="C3" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
     </row>
     <row r="4" spans="2:9" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="32"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="29"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="25"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
     </row>
     <row r="5" spans="2:9" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="33"/>
-      <c r="C5" s="26" t="s">
+      <c r="B5" s="29"/>
+      <c r="C5" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
       <c r="I5" s="15"/>
     </row>
     <row r="6" spans="2:9" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="33"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="33"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="29"/>
       <c r="E6" s="19"/>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
@@ -1479,9 +1482,9 @@
       <c r="I6" s="15"/>
     </row>
     <row r="7" spans="2:9" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="33"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="33"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="29"/>
       <c r="E7" s="19"/>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
@@ -1489,9 +1492,9 @@
       <c r="I7" s="15"/>
     </row>
     <row r="8" spans="2:9" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="33"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="33"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="29"/>
       <c r="E8" s="19"/>
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
@@ -1499,9 +1502,9 @@
       <c r="I8" s="15"/>
     </row>
     <row r="9" spans="2:9" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="33"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="33"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="29"/>
       <c r="E9" s="19"/>
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
@@ -1509,9 +1512,9 @@
       <c r="I9" s="15"/>
     </row>
     <row r="10" spans="2:9" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="33"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="33"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="29"/>
       <c r="E10" s="19"/>
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
@@ -1519,9 +1522,9 @@
       <c r="I10" s="15"/>
     </row>
     <row r="11" spans="2:9" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="33"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="33"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="29"/>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
@@ -1529,9 +1532,9 @@
       <c r="I11" s="15"/>
     </row>
     <row r="12" spans="2:9" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="33"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="33"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="29"/>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
@@ -1539,9 +1542,9 @@
       <c r="I12" s="15"/>
     </row>
     <row r="13" spans="2:9" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="33"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="33"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="29"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
@@ -1620,7 +1623,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C3" sqref="C3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1668,19 +1671,19 @@
     </row>
     <row r="5" spans="2:8" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="14"/>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="36" t="s">
         <v>11</v>
       </c>
       <c r="H5" s="14"/>
@@ -1709,12 +1712,12 @@
       <c r="E8"/>
     </row>
     <row r="9" spans="2:8" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="24"/>
+      <c r="B9" s="20"/>
     </row>
     <row r="10" spans="2:8" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="2:8" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="2:8" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D12" s="24"/>
+      <c r="D12" s="20"/>
     </row>
     <row r="13" spans="2:8" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="2:8" ht="28" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>